<commit_message>
Szenarien entwickelt, Formattierung Konsistenzmatrix
</commit_message>
<xml_diff>
--- a/Meilenstein 1/Dokumente/Konsistenzmatrix.xlsx
+++ b/Meilenstein 1/Dokumente/Konsistenzmatrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\GitHub\MKon\Meilenstein 1\Dokumente klatte 04.11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\GitHub\MKon\Meilenstein 1\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB914FA7-BB2C-4007-85B7-B1ED6D5660D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E211C6AA-7D11-4E9A-9B61-E6FC863BAAA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{03134C5B-0C5B-4803-A455-FECFDAF53424}"/>
   </bookViews>
@@ -435,27 +435,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,20 +509,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -494,31 +516,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -836,7 +848,7 @@
   <dimension ref="B2:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,24 +862,24 @@
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="17" t="s">
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -876,14 +888,14 @@
     </row>
     <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="C4" s="15"/>
+      <c r="D4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6">
         <v>0</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -895,18 +907,18 @@
       <c r="I4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="9">
+      <c r="J4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -914,22 +926,22 @@
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="23"/>
-      <c r="N5" s="11" t="s">
+      <c r="C5" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="13"/>
+      <c r="N5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="O5" s="1"/>
@@ -940,21 +952,21 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
-      <c r="C6" s="8">
+      <c r="B6" s="35"/>
+      <c r="C6" s="38">
         <v>0</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="23"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="13"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="O6" s="1"/>
@@ -965,21 +977,21 @@
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="35"/>
+      <c r="C7" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="23"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="13"/>
+      <c r="N7" s="9"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -987,29 +999,29 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="C8" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="16">
         <v>9</v>
       </c>
-      <c r="E8" s="10">
-        <v>5</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="E8" s="16">
+        <v>5</v>
+      </c>
+      <c r="F8" s="16">
         <v>0</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="23"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="10" t="s">
         <v>9</v>
       </c>
       <c r="O8" s="1"/>
@@ -1020,27 +1032,27 @@
       <c r="T8" s="1"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
-      <c r="C9" s="3">
+      <c r="B9" s="26"/>
+      <c r="C9" s="39">
         <v>0</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="16">
         <v>7</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="16">
         <v>9</v>
       </c>
-      <c r="F9" s="10">
-        <v>5</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="23"/>
+      <c r="F9" s="16">
+        <v>5</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="14" t="s">
+      <c r="N9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="O9" s="1"/>
@@ -1051,27 +1063,27 @@
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="34"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="36"/>
+      <c r="C10" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="16">
         <v>3</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="16">
         <v>7</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="16">
         <v>9</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="23"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="15" t="s">
+      <c r="N10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="O10" s="1"/>
@@ -1082,10 +1094,10 @@
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6">
@@ -1097,18 +1109,18 @@
       <c r="F11" s="6">
         <v>5</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="16">
         <v>9</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="16">
         <v>7</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="16">
         <v>3</v>
       </c>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="23"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="18"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1119,8 +1131,8 @@
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
-      <c r="C12" s="8">
+      <c r="B12" s="23"/>
+      <c r="C12" s="38">
         <v>0</v>
       </c>
       <c r="D12" s="6">
@@ -1132,18 +1144,18 @@
       <c r="F12" s="6">
         <v>5</v>
       </c>
-      <c r="G12" s="10">
-        <v>5</v>
-      </c>
-      <c r="H12" s="10">
-        <v>5</v>
-      </c>
-      <c r="I12" s="10">
-        <v>5</v>
-      </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="23"/>
+      <c r="G12" s="16">
+        <v>5</v>
+      </c>
+      <c r="H12" s="16">
+        <v>5</v>
+      </c>
+      <c r="I12" s="16">
+        <v>5</v>
+      </c>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="18"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1154,8 +1166,8 @@
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="37"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="38" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="6">
@@ -1167,18 +1179,18 @@
       <c r="F13" s="6">
         <v>9</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="16">
         <v>0</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="16">
         <v>3</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="16">
         <v>3</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="23"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="18"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1189,10 +1201,10 @@
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="39" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="6">
@@ -1204,13 +1216,13 @@
       <c r="F14" s="6">
         <v>9</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="16">
         <v>3</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="16">
         <v>7</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="16">
         <v>9</v>
       </c>
       <c r="J14" s="6">
@@ -1219,7 +1231,7 @@
       <c r="K14" s="6">
         <v>5</v>
       </c>
-      <c r="L14" s="24">
+      <c r="L14" s="12">
         <v>0</v>
       </c>
       <c r="M14" s="1"/>
@@ -1232,8 +1244,8 @@
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="33"/>
-      <c r="C15" s="3">
+      <c r="B15" s="26"/>
+      <c r="C15" s="39">
         <v>0</v>
       </c>
       <c r="D15" s="6">
@@ -1245,13 +1257,13 @@
       <c r="F15" s="6">
         <v>5</v>
       </c>
-      <c r="G15" s="10">
-        <v>5</v>
-      </c>
-      <c r="H15" s="10">
+      <c r="G15" s="16">
+        <v>5</v>
+      </c>
+      <c r="H15" s="16">
         <v>9</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="16">
         <v>9</v>
       </c>
       <c r="J15" s="6">
@@ -1260,7 +1272,7 @@
       <c r="K15" s="6">
         <v>5</v>
       </c>
-      <c r="L15" s="24">
+      <c r="L15" s="12">
         <v>3</v>
       </c>
       <c r="M15" s="1"/>
@@ -1273,35 +1285,35 @@
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="28" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="19">
         <v>9</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="19">
         <v>7</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="19">
         <v>3</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="20">
         <v>9</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="20">
         <v>3</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="20">
         <v>3</v>
       </c>
-      <c r="J16" s="25">
-        <v>5</v>
-      </c>
-      <c r="K16" s="25">
+      <c r="J16" s="19">
+        <v>5</v>
+      </c>
+      <c r="K16" s="19">
         <v>7</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="21">
         <v>9</v>
       </c>
       <c r="M16" s="1"/>

</xml_diff>